<commit_message>
representacion de instrucciones y reglas2
</commit_message>
<xml_diff>
--- a/Representacion de Instrucciones y Reglas.xlsx
+++ b/Representacion de Instrucciones y Reglas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Instrucciones del juego Clue</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t xml:space="preserve">El sistemas tomara el puesto del usuario que perdio para seguir tratando de probar que las sugerencias de sus oponentes son falsas al enseñar los naipes cuando sea solicitado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sus oponentes pueden seguir moviendo su peón a los  distintos aposentos donde ellos hagan las sugerencias </t>
+  </si>
+  <si>
+    <t>Si, al hacer una acusación falsa, su peón está bloqueando una puerta, muévalo dentro del aposento para permitir el paso a los jugadores restantes</t>
+  </si>
+  <si>
+    <t>Si, al hacer una acusación falsa, su peón está bloqueando una puerta, el sistema movera su peón dentro del aposento</t>
   </si>
 </sst>
 </file>
@@ -684,7 +693,7 @@
   <dimension ref="C1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,65 +1359,64 @@
       <c r="C42" s="3">
         <v>37</v>
       </c>
-      <c r="D42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
+      <c r="H42" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
     <row r="43" spans="3:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="3">
+        <v>38</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
+      <c r="H43" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="D42:G42"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="D39:G39"/>
@@ -1425,33 +1433,44 @@
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="D35:G35"/>
     <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
     <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="H43:K43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
final representacion de instrucciones
</commit_message>
<xml_diff>
--- a/Representacion de Instrucciones y Reglas.xlsx
+++ b/Representacion de Instrucciones y Reglas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Instrucciones del juego Clue</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Si, al hacer una acusación falsa, su peón está bloqueando una puerta, el sistema movera su peón dentro del aposento</t>
+  </si>
+  <si>
+    <t>Ganando. Gana el jugador cuya acusación es completamente verdadera- es decir, el que encuentra en el sobre los tres naipes y muestralos  a todos los jugadores.</t>
+  </si>
+  <si>
+    <t>Ganando. Gana el jugador cuya acusación es completamente verdadera- es decir, el que encuentra en el sobre los tres naipes, el sistema les mostrara los naipes a todos los jugadores.</t>
   </si>
 </sst>
 </file>
@@ -690,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:L43"/>
+  <dimension ref="C1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,8 +1395,27 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
+    <row r="44" spans="3:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="3">
+        <v>39</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="82">
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="H44:K44"/>
     <mergeCell ref="H37:K37"/>
     <mergeCell ref="H38:K38"/>
     <mergeCell ref="H39:K39"/>

</xml_diff>